<commit_message>
Auto upercase, Eyes, Outbox != '', Inbox = '', Update frontend
</commit_message>
<xml_diff>
--- a/data_user.xlsx
+++ b/data_user.xlsx
@@ -1,26 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
-  <workbookPr codeName="ThisWorkbook"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27029"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\approval_app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3761A02E-888F-43E8-9FE6-358FDFA469C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{941971FE-7E00-40BC-864C-B188AED75394}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Name</t>
   </si>
@@ -31,25 +44,16 @@
     <t>VANCHIEN</t>
   </si>
   <si>
-    <t>IEN2UIGO75VANCHI</t>
-  </si>
-  <si>
     <t>THANHTRUNG</t>
   </si>
   <si>
-    <t>UNG2UIGO75THANHT</t>
-  </si>
-  <si>
     <t>HUUTHUAN</t>
   </si>
   <si>
-    <t>UAN2UIGO75HUUTHU</t>
-  </si>
-  <si>
-    <t>phamhuy</t>
-  </si>
-  <si>
-    <t>HUY2UIGO75PHAMHU</t>
+    <t>PHANLINH</t>
+  </si>
+  <si>
+    <t>PHAMHUY</t>
   </si>
 </sst>
 </file>
@@ -58,22 +62,22 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="12"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="10"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
-      <b/>
       <sz val="10"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -86,7 +90,14 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left/>
       <right/>
@@ -98,16 +109,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -253,7 +271,6 @@
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
                 <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
@@ -264,27 +281,31 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="100000"/>
-                <a:shade val="100000"/>
+                <a:tint val="51000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:shade val="100000"/>
-                <a:satMod val="350000"/>
+                <a:tint val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
         <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
+              <a:shade val="9500"/>
               <a:satMod val="105000"/>
             </a:schemeClr>
           </a:solidFill>
@@ -306,7 +327,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -364,7 +385,7 @@
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
+                <a:tint val="20000"/>
                 <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
@@ -377,13 +398,12 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
                 <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
                 <a:satMod val="200000"/>
               </a:schemeClr>
             </a:gs>
@@ -395,108 +415,82 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults>
-    <a:spDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="3">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </a:style>
-    </a:spDef>
-    <a:lnDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </a:style>
-    </a:lnDef>
-  </a:objectDefaults>
+  <a:objectDefaults/>
   <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B5"/>
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="str">
+        <f t="shared" ref="B2:B6" si="0">RIGHT(A2,3)&amp;"2UIGO75"&amp;LEFT(A2,6)</f>
+        <v>IEN2UIGO75VANCHI</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="B3" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>UNG2UIGO75THANHT</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B4" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>UAN2UIGO75HUUTHU</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+      <c r="B5" s="2" t="str">
+        <f>RIGHT(A5,3)&amp;"2UIGO75"&amp;LEFT(A5,6)</f>
+        <v>INH2UIGO75PHANLI</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>9</v>
+      <c r="B6" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>HUY2UIGO75PHAMHU</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <ignoredErrors>
-    <ignoredError sqref="A1:B5" numberStoredAsText="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>